<commit_message>
Asignación de nivel al cargue por jupyter y pandas
</commit_message>
<xml_diff>
--- a/logistica/cargue.xlsx
+++ b/logistica/cargue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProyectosWeb\assigment\logistica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB42340B-9062-4182-BB90-3AE19AF0E19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E90956-EE47-4A96-ABDA-3BF83B62DB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{487DD5BE-BA3A-4526-BABC-C231642C0B8F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
   <si>
     <t>Descripción</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>Total Entrega</t>
-  </si>
-  <si>
-    <t>19071</t>
   </si>
   <si>
     <t>BON BON BUM FRESA INTENSA*24 UND</t>
@@ -309,8 +306,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,14 +626,14 @@
   <dimension ref="A1:AF36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -660,7 +658,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -695,11 +693,11 @@
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1">
+        <v>19071</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
       </c>
       <c r="T6">
         <v>15</v>
@@ -716,10 +714,10 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
         <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
       </c>
       <c r="T7">
         <v>15</v>
@@ -736,10 +734,10 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
       </c>
       <c r="T8">
         <v>24</v>
@@ -756,16 +754,16 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
         <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
       </c>
       <c r="T9">
         <v>4</v>
       </c>
       <c r="Y9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AA9">
         <v>4863.6728000000003</v>
@@ -776,16 +774,16 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
         <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
       </c>
       <c r="T10">
         <v>4</v>
       </c>
       <c r="Y10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AA10">
         <v>4667.9178000000002</v>
@@ -796,16 +794,16 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
         <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
       </c>
       <c r="T11">
         <v>4</v>
       </c>
       <c r="Y11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AA11">
         <v>7075.1450000000004</v>
@@ -816,16 +814,16 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
         <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
       </c>
       <c r="T12">
         <v>10</v>
       </c>
       <c r="Y12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AA12">
         <v>5727.232</v>
@@ -836,16 +834,16 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
         <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
       </c>
       <c r="T13">
         <v>9</v>
       </c>
       <c r="Y13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AA13">
         <v>7131.0749999999998</v>
@@ -856,16 +854,16 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
         <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
       </c>
       <c r="T14">
         <v>9</v>
       </c>
       <c r="Y14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AA14">
         <v>4222.7150000000001</v>
@@ -876,16 +874,16 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
         <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>30</v>
       </c>
       <c r="T15">
         <v>8</v>
       </c>
       <c r="Y15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA15">
         <v>5949.8334000000004</v>
@@ -896,16 +894,16 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
         <v>32</v>
-      </c>
-      <c r="C16" t="s">
-        <v>33</v>
       </c>
       <c r="T16">
         <v>8</v>
       </c>
       <c r="Y16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA16">
         <v>6222.7718000000004</v>
@@ -916,10 +914,10 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
         <v>34</v>
-      </c>
-      <c r="C17" t="s">
-        <v>35</v>
       </c>
       <c r="T17">
         <v>12</v>
@@ -936,16 +934,16 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
         <v>36</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
       </c>
       <c r="T18">
         <v>1</v>
       </c>
       <c r="Y18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AA18">
         <v>8107.6127999999999</v>
@@ -956,16 +954,16 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
         <v>39</v>
-      </c>
-      <c r="C19" t="s">
-        <v>40</v>
       </c>
       <c r="T19">
         <v>4</v>
       </c>
       <c r="Y19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AA19">
         <v>5726.1134000000002</v>
@@ -976,16 +974,16 @@
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
         <v>41</v>
-      </c>
-      <c r="C20" t="s">
-        <v>42</v>
       </c>
       <c r="T20">
         <v>4</v>
       </c>
       <c r="Y20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AA20">
         <v>5726.1134000000002</v>
@@ -996,16 +994,16 @@
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
         <v>43</v>
-      </c>
-      <c r="C21" t="s">
-        <v>44</v>
       </c>
       <c r="T21">
         <v>2</v>
       </c>
       <c r="Y21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA21">
         <v>5463.2424000000001</v>
@@ -1016,16 +1014,16 @@
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
         <v>46</v>
-      </c>
-      <c r="C22" t="s">
-        <v>47</v>
       </c>
       <c r="T22">
         <v>2</v>
       </c>
       <c r="Y22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA22">
         <v>5463.2424000000001</v>
@@ -1036,16 +1034,16 @@
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
         <v>48</v>
-      </c>
-      <c r="C23" t="s">
-        <v>49</v>
       </c>
       <c r="T23">
         <v>3</v>
       </c>
       <c r="Y23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AA23">
         <v>5463.2424000000001</v>
@@ -1056,16 +1054,16 @@
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" t="s">
         <v>51</v>
-      </c>
-      <c r="C24" t="s">
-        <v>52</v>
       </c>
       <c r="T24">
         <v>3</v>
       </c>
       <c r="Y24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AA24">
         <v>5463.2424000000001</v>
@@ -1076,10 +1074,10 @@
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
         <v>53</v>
-      </c>
-      <c r="C25" t="s">
-        <v>54</v>
       </c>
       <c r="T25">
         <v>30</v>
@@ -1096,10 +1094,10 @@
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
         <v>55</v>
-      </c>
-      <c r="C26" t="s">
-        <v>56</v>
       </c>
       <c r="T26">
         <v>16</v>
@@ -1116,16 +1114,16 @@
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
         <v>57</v>
-      </c>
-      <c r="C27" t="s">
-        <v>58</v>
       </c>
       <c r="T27">
         <v>10</v>
       </c>
       <c r="Y27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AA27">
         <v>3237.2284</v>
@@ -1136,16 +1134,16 @@
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
         <v>59</v>
-      </c>
-      <c r="C28" t="s">
-        <v>60</v>
       </c>
       <c r="T28">
         <v>10</v>
       </c>
       <c r="Y28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AA28">
         <v>6361.4781999999996</v>
@@ -1156,16 +1154,16 @@
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
         <v>61</v>
-      </c>
-      <c r="C29" t="s">
-        <v>62</v>
       </c>
       <c r="T29">
         <v>12</v>
       </c>
       <c r="Y29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA29">
         <v>733.80160000000001</v>
@@ -1176,16 +1174,16 @@
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" t="s">
         <v>64</v>
-      </c>
-      <c r="C30" t="s">
-        <v>65</v>
       </c>
       <c r="T30">
         <v>2</v>
       </c>
       <c r="Y30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA30">
         <v>11731.8768</v>
@@ -1196,16 +1194,16 @@
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" t="s">
         <v>66</v>
-      </c>
-      <c r="C31" t="s">
-        <v>67</v>
       </c>
       <c r="T31">
         <v>8</v>
       </c>
       <c r="Y31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA31">
         <v>6349.1736000000001</v>
@@ -1216,16 +1214,16 @@
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" t="s">
         <v>68</v>
-      </c>
-      <c r="C32" t="s">
-        <v>69</v>
       </c>
       <c r="T32">
         <v>4</v>
       </c>
       <c r="Y32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AA32">
         <v>10297.8316</v>
@@ -1236,16 +1234,16 @@
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" t="s">
         <v>70</v>
-      </c>
-      <c r="C33" t="s">
-        <v>71</v>
       </c>
       <c r="T33">
         <v>4</v>
       </c>
       <c r="Y33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AA33">
         <v>10297.8316</v>
@@ -1256,16 +1254,16 @@
     </row>
     <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" t="s">
         <v>72</v>
-      </c>
-      <c r="C34" t="s">
-        <v>73</v>
       </c>
       <c r="T34">
         <v>5</v>
       </c>
       <c r="Y34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA34">
         <v>3660.0592000000001</v>
@@ -1276,16 +1274,16 @@
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" t="s">
         <v>75</v>
-      </c>
-      <c r="C35" t="s">
-        <v>76</v>
       </c>
       <c r="T35">
         <v>5</v>
       </c>
       <c r="Y35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA35">
         <v>4771.9476000000004</v>
@@ -1296,16 +1294,16 @@
     </row>
     <row r="36" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" t="s">
         <v>77</v>
-      </c>
-      <c r="C36" t="s">
-        <v>78</v>
       </c>
       <c r="T36">
         <v>5</v>
       </c>
       <c r="Y36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA36">
         <v>4771.9476000000004</v>

</xml_diff>

<commit_message>
Todos los codigos identificados, inicio proceso limpiar base de datos cargue
</commit_message>
<xml_diff>
--- a/logistica/cargue.xlsx
+++ b/logistica/cargue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProyectosWeb\assigment\logistica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E90956-EE47-4A96-ABDA-3BF83B62DB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EC2E1C-2590-4D20-A38B-B1C905FB7BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{487DD5BE-BA3A-4526-BABC-C231642C0B8F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
   <si>
     <t>Descripción</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Precio</t>
-  </si>
-  <si>
-    <t>ALDOR</t>
   </si>
   <si>
     <t>TROLLI GOMAS MAGENTA SUR*24 BANAN-MORDISC+OINK+EMOCION</t>
@@ -626,14 +623,14 @@
   <dimension ref="A1:AF36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -652,22 +649,22 @@
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
+      <c r="A2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T3">
         <v>1</v>
       </c>
       <c r="Y3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AA3">
         <v>21432.376</v>
@@ -681,7 +678,7 @@
         <v>1218</v>
       </c>
       <c r="X4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AB4">
         <v>21432.376</v>
@@ -697,13 +694,13 @@
         <v>19071</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T6">
         <v>15</v>
       </c>
       <c r="Y6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AA6">
         <v>6049.7835990000003</v>
@@ -714,16 +711,16 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
         <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
       </c>
       <c r="T7">
         <v>15</v>
       </c>
       <c r="Y7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AA7">
         <v>6049.7835990000003</v>
@@ -734,16 +731,16 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
         <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
       </c>
       <c r="T8">
         <v>24</v>
       </c>
       <c r="Y8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AA8">
         <v>4317.7960000000003</v>
@@ -754,16 +751,16 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
         <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
       </c>
       <c r="T9">
         <v>4</v>
       </c>
       <c r="Y9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA9">
         <v>4863.6728000000003</v>
@@ -774,16 +771,16 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
         <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
       </c>
       <c r="T10">
         <v>4</v>
       </c>
       <c r="Y10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA10">
         <v>4667.9178000000002</v>
@@ -794,16 +791,16 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
         <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
       </c>
       <c r="T11">
         <v>4</v>
       </c>
       <c r="Y11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA11">
         <v>7075.1450000000004</v>
@@ -814,16 +811,16 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
         <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
       </c>
       <c r="T12">
         <v>10</v>
       </c>
       <c r="Y12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA12">
         <v>5727.232</v>
@@ -834,16 +831,16 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
         <v>23</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
       </c>
       <c r="T13">
         <v>9</v>
       </c>
       <c r="Y13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AA13">
         <v>7131.0749999999998</v>
@@ -854,16 +851,16 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
         <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>27</v>
       </c>
       <c r="T14">
         <v>9</v>
       </c>
       <c r="Y14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AA14">
         <v>4222.7150000000001</v>
@@ -874,16 +871,16 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
         <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
       </c>
       <c r="T15">
         <v>8</v>
       </c>
       <c r="Y15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AA15">
         <v>5949.8334000000004</v>
@@ -894,16 +891,16 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
         <v>31</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
       </c>
       <c r="T16">
         <v>8</v>
       </c>
       <c r="Y16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AA16">
         <v>6222.7718000000004</v>
@@ -914,16 +911,16 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
         <v>33</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
       </c>
       <c r="T17">
         <v>12</v>
       </c>
       <c r="Y17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AA17">
         <v>9273.1939999999995</v>
@@ -934,16 +931,16 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
         <v>35</v>
-      </c>
-      <c r="C18" t="s">
-        <v>36</v>
       </c>
       <c r="T18">
         <v>1</v>
       </c>
       <c r="Y18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AA18">
         <v>8107.6127999999999</v>
@@ -954,16 +951,16 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
         <v>38</v>
-      </c>
-      <c r="C19" t="s">
-        <v>39</v>
       </c>
       <c r="T19">
         <v>4</v>
       </c>
       <c r="Y19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA19">
         <v>5726.1134000000002</v>
@@ -974,16 +971,16 @@
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
         <v>40</v>
-      </c>
-      <c r="C20" t="s">
-        <v>41</v>
       </c>
       <c r="T20">
         <v>4</v>
       </c>
       <c r="Y20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA20">
         <v>5726.1134000000002</v>
@@ -994,16 +991,16 @@
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
         <v>42</v>
-      </c>
-      <c r="C21" t="s">
-        <v>43</v>
       </c>
       <c r="T21">
         <v>2</v>
       </c>
       <c r="Y21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AA21">
         <v>5463.2424000000001</v>
@@ -1014,16 +1011,16 @@
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
         <v>45</v>
-      </c>
-      <c r="C22" t="s">
-        <v>46</v>
       </c>
       <c r="T22">
         <v>2</v>
       </c>
       <c r="Y22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AA22">
         <v>5463.2424000000001</v>
@@ -1034,16 +1031,16 @@
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
         <v>47</v>
-      </c>
-      <c r="C23" t="s">
-        <v>48</v>
       </c>
       <c r="T23">
         <v>3</v>
       </c>
       <c r="Y23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AA23">
         <v>5463.2424000000001</v>
@@ -1054,16 +1051,16 @@
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
         <v>50</v>
-      </c>
-      <c r="C24" t="s">
-        <v>51</v>
       </c>
       <c r="T24">
         <v>3</v>
       </c>
       <c r="Y24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AA24">
         <v>5463.2424000000001</v>
@@ -1074,16 +1071,16 @@
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
         <v>52</v>
-      </c>
-      <c r="C25" t="s">
-        <v>53</v>
       </c>
       <c r="T25">
         <v>30</v>
       </c>
       <c r="Y25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AA25">
         <v>3166.7566000000002</v>
@@ -1094,16 +1091,16 @@
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
         <v>54</v>
-      </c>
-      <c r="C26" t="s">
-        <v>55</v>
       </c>
       <c r="T26">
         <v>16</v>
       </c>
       <c r="Y26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AA26">
         <v>7607.5986000000003</v>
@@ -1114,16 +1111,16 @@
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
         <v>56</v>
-      </c>
-      <c r="C27" t="s">
-        <v>57</v>
       </c>
       <c r="T27">
         <v>10</v>
       </c>
       <c r="Y27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA27">
         <v>3237.2284</v>
@@ -1134,16 +1131,16 @@
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" t="s">
         <v>58</v>
-      </c>
-      <c r="C28" t="s">
-        <v>59</v>
       </c>
       <c r="T28">
         <v>10</v>
       </c>
       <c r="Y28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA28">
         <v>6361.4781999999996</v>
@@ -1154,16 +1151,16 @@
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
         <v>60</v>
-      </c>
-      <c r="C29" t="s">
-        <v>61</v>
       </c>
       <c r="T29">
         <v>12</v>
       </c>
       <c r="Y29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AA29">
         <v>733.80160000000001</v>
@@ -1174,16 +1171,16 @@
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
         <v>63</v>
-      </c>
-      <c r="C30" t="s">
-        <v>64</v>
       </c>
       <c r="T30">
         <v>2</v>
       </c>
       <c r="Y30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AA30">
         <v>11731.8768</v>
@@ -1194,16 +1191,16 @@
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
         <v>65</v>
-      </c>
-      <c r="C31" t="s">
-        <v>66</v>
       </c>
       <c r="T31">
         <v>8</v>
       </c>
       <c r="Y31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AA31">
         <v>6349.1736000000001</v>
@@ -1214,16 +1211,16 @@
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" t="s">
         <v>67</v>
-      </c>
-      <c r="C32" t="s">
-        <v>68</v>
       </c>
       <c r="T32">
         <v>4</v>
       </c>
       <c r="Y32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA32">
         <v>10297.8316</v>
@@ -1234,16 +1231,16 @@
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
         <v>69</v>
-      </c>
-      <c r="C33" t="s">
-        <v>70</v>
       </c>
       <c r="T33">
         <v>4</v>
       </c>
       <c r="Y33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA33">
         <v>10297.8316</v>
@@ -1254,16 +1251,16 @@
     </row>
     <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="s">
         <v>71</v>
-      </c>
-      <c r="C34" t="s">
-        <v>72</v>
       </c>
       <c r="T34">
         <v>5</v>
       </c>
       <c r="Y34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AA34">
         <v>3660.0592000000001</v>
@@ -1274,16 +1271,16 @@
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" t="s">
         <v>74</v>
-      </c>
-      <c r="C35" t="s">
-        <v>75</v>
       </c>
       <c r="T35">
         <v>5</v>
       </c>
       <c r="Y35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AA35">
         <v>4771.9476000000004</v>
@@ -1294,16 +1291,16 @@
     </row>
     <row r="36" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" t="s">
         <v>76</v>
-      </c>
-      <c r="C36" t="s">
-        <v>77</v>
       </c>
       <c r="T36">
         <v>5</v>
       </c>
       <c r="Y36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AA36">
         <v>4771.9476000000004</v>

</xml_diff>

<commit_message>
Se unifican tablas eliminando Unnamed
</commit_message>
<xml_diff>
--- a/logistica/cargue.xlsx
+++ b/logistica/cargue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProyectosWeb\assigment\logistica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EC2E1C-2590-4D20-A38B-B1C905FB7BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7E3A07-69A3-4BC7-8972-B4C534452B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{487DD5BE-BA3A-4526-BABC-C231642C0B8F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="78">
   <si>
     <t>Descripción</t>
   </si>
@@ -267,9 +267,6 @@
   </si>
   <si>
     <t>Codigo</t>
-  </si>
-  <si>
-    <t>A</t>
   </si>
 </sst>
 </file>
@@ -622,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44158381-E68A-43A7-8D84-6BE4411C4E5E}">
   <dimension ref="A1:AF36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -655,7 +652,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Base de datos sin datos na ni texto
</commit_message>
<xml_diff>
--- a/logistica/cargue.xlsx
+++ b/logistica/cargue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProyectosWeb\assigment\logistica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0915EF1A-CD19-4586-819B-BF36F770DD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44276DFC-D678-43EB-A09E-7ED16DB79A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9BC25289-FCA6-4F49-AC5D-3FADFA3753A0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="514">
   <si>
     <t>Descripción</t>
   </si>
@@ -1572,27 +1572,6 @@
   </si>
   <si>
     <t>VELON BLANCO 02 *12 PEQ</t>
-  </si>
-  <si>
-    <t>Asesores</t>
-  </si>
-  <si>
-    <t>Telefono</t>
-  </si>
-  <si>
-    <t>Cantidad</t>
-  </si>
-  <si>
-    <t>JOSE DAVID CALDERON CASAS</t>
-  </si>
-  <si>
-    <t>3177309102</t>
-  </si>
-  <si>
-    <t>JEISSON HERNANDO GARCIA</t>
-  </si>
-  <si>
-    <t>3155152244</t>
   </si>
   <si>
     <t>Codigo</t>
@@ -1947,17 +1926,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8EA2C0-375B-419A-9E83-8A98608339E7}">
-  <dimension ref="A1:AF270"/>
+  <dimension ref="A1:AF266"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
+      <selection activeCell="K267" sqref="K267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -6814,39 +6793,6 @@
       </c>
       <c r="AB266">
         <v>41255.514999999999</v>
-      </c>
-    </row>
-    <row r="268" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A268" t="s">
-        <v>513</v>
-      </c>
-      <c r="L268" t="s">
-        <v>514</v>
-      </c>
-      <c r="M268" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="269" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A269" t="s">
-        <v>516</v>
-      </c>
-      <c r="L269" t="s">
-        <v>517</v>
-      </c>
-      <c r="M269">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="270" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A270" t="s">
-        <v>518</v>
-      </c>
-      <c r="L270" t="s">
-        <v>519</v>
-      </c>
-      <c r="M270">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>